<commit_message>
modificato scarico per calcolare valori batch
</commit_message>
<xml_diff>
--- a/reports e riferimenti/MSQ.xlsx
+++ b/reports e riferimenti/MSQ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/michele_tosi_students_uniroma2_eu/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/michele_tosi_students_uniroma2_eu/Documents/Desktop/PMCSN/AMA-ROMA_PMCSN/reports e riferimenti/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96754257-0EBA-48EA-AA7F-78DE3853AF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{96754257-0EBA-48EA-AA7F-78DE3853AF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E997F3F-78B9-40AE-9DF2-B0FCFDC2CB6A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{0A54CB1D-96A8-4DA3-B11B-B6CFD14F36F1}"/>
   </bookViews>
@@ -468,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.3">
@@ -483,14 +483,14 @@
       </c>
       <c r="D3">
         <f>+B3/B2</f>
-        <v>150</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F3">
         <f>1/D3</f>
-        <v>6.6666666666666671E-3</v>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.3">
@@ -499,7 +499,7 @@
       </c>
       <c r="B4">
         <f>(B1*D1)/F3</f>
-        <v>0.24749999999999994</v>
+        <v>9.8999999999999991E-2</v>
       </c>
       <c r="K4" t="s">
         <v>8</v>
@@ -511,7 +511,7 @@
       </c>
       <c r="B5">
         <f>(+SUM(K5:Z5)+(B2*B4)^B2/(FACT(B2)*(1-B4)))^(-1)</f>
-        <v>0.37106362058362646</v>
+        <v>0.37157669061446941</v>
       </c>
       <c r="K5">
         <f>($B$2*$B$4)^K6/FACT(K6)</f>
@@ -519,39 +519,39 @@
       </c>
       <c r="L5">
         <f>IF(L6&lt;&gt;0,(($B$2*$B$4)^L6/(FACT(L6))),0)</f>
-        <v>0.98999999999999977</v>
+        <v>0.98999999999999988</v>
       </c>
       <c r="M5">
         <f t="shared" ref="M5:Z5" si="0">IF(M6&lt;&gt;0,(($B$2*$B$4)^M6/(FACT(M6))),0)</f>
-        <v>0.49004999999999976</v>
+        <v>0.49004999999999987</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>0.1617164999999999</v>
+        <v>0.16171649999999996</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.0024833749999982E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.9249170824999948E-3</v>
       </c>
       <c r="Q5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.307611318612499E-3</v>
       </c>
       <c r="R5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.8493360077519627E-4</v>
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2885533095930537E-5</v>
       </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.5174086405523585E-6</v>
       </c>
       <c r="U5">
         <f t="shared" si="0"/>
@@ -584,7 +584,7 @@
       </c>
       <c r="B6">
         <f>+(B2*B4)^4*B5/(FACT(B2)*(1-B4))</f>
-        <v>1.9736557773465398E-2</v>
+        <v>1.0916952406804987E-7</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -593,7 +593,7 @@
         <v>1</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="L6:N6" si="1">+IF(AND($B$2&gt;L6+1,L6+1&lt;&gt;1),L6+1,0)</f>
+        <f t="shared" ref="M6:N6" si="1">+IF(AND($B$2&gt;L6+1,L6+1&lt;&gt;1),L6+1,0)</f>
         <v>2</v>
       </c>
       <c r="N6">
@@ -602,27 +602,27 @@
       </c>
       <c r="O6">
         <f>+IF(AND($B$2&gt;N6+1,N6+1&lt;&gt;1),N6+1,0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="P6">
         <f t="shared" ref="P6:Z6" si="2">+IF(AND($B$2&gt;O6+1,O6+1&lt;&gt;1),O6+1,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U6">
         <f t="shared" si="2"/>
@@ -655,14 +655,14 @@
       </c>
       <c r="B7">
         <f>+(B6*D3)/(1-B4)</f>
-        <v>3.9341975628170225</v>
+        <v>7.2698906149644746E-6</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7">
         <f>+B7+B3</f>
-        <v>603.93419756281708</v>
+        <v>600.0000072698906</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
@@ -671,14 +671,14 @@
       </c>
       <c r="B8">
         <f>+B7*B1*D1</f>
-        <v>6.4914259786480874E-3</v>
+        <v>1.1995319514691381E-8</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
       <c r="D8">
         <f>+D7*B1*D1</f>
-        <v>0.99649142597864804</v>
+        <v>0.9900000119953194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrette formule Msq per coda M/M/1
</commit_message>
<xml_diff>
--- a/reports e riferimenti/MSQ.xlsx
+++ b/reports e riferimenti/MSQ.xlsx
@@ -724,7 +724,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="71" workbookViewId="0">
+    <sheetView topLeftCell="A82" zoomScale="71" workbookViewId="0">
       <selection activeCell="D87" activeCellId="0" sqref="D87"/>
     </sheetView>
   </sheetViews>
@@ -1249,21 +1249,21 @@
         <v>4</v>
       </c>
       <c r="B28">
-        <v>5400</v>
+        <v>3600</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D28">
         <f>+B28/B27</f>
-        <v>1800</v>
+        <v>1200</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>0.00055555555555555556</v>
+        <v>0.00083333333333333339</v>
       </c>
     </row>
     <row r="29">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="B29" s="6">
         <f>(B26*D26)/F28</f>
-        <v>0.89099999999999979</v>
+        <v>0.59399999999999986</v>
       </c>
       <c r="K29" t="s">
         <v>8</v>
@@ -1284,7 +1284,7 @@
       </c>
       <c r="B30">
         <f>(+SUM(K30:Z30)+(B27*B29)^B27/(FACT(B27)*(1-B29)))^(-1)</f>
-        <v>0.027436420186509831</v>
+        <v>0.14941554966889375</v>
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
@@ -1292,11 +1292,11 @@
       </c>
       <c r="L30">
         <f t="shared" si="4"/>
-        <v>2.6729999999999992</v>
+        <v>1.7819999999999996</v>
       </c>
       <c r="M30">
         <f t="shared" si="4"/>
-        <v>3.5724644999999979</v>
+        <v>1.5877619999999992</v>
       </c>
       <c r="N30">
         <f>IF(N31&lt;&gt;0,(($B27*$B29)^N31/(FACT(N31))),0)</f>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B31">
         <f>+(B27*B29)^B27*B30/(FACT(B27)*(1-B29))</f>
-        <v>0.80121039153155982</v>
+        <v>0.34708960884775569</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -1428,14 +1428,14 @@
       </c>
       <c r="B32" s="6">
         <f>+(B31*D28)/(1-B29)</f>
-        <v>13230.997291346835</v>
+        <v>1025.8806172840066</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D32" s="6">
         <f>+B32+B28</f>
-        <v>18630.997291346837</v>
+        <v>4625.8806172840068</v>
       </c>
     </row>
     <row r="33">
@@ -1444,14 +1444,14 @@
       </c>
       <c r="B33" s="6">
         <f>+B32*B26*D26</f>
-        <v>6.5493436592166825</v>
+        <v>0.50781090555558317</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D33" s="6">
         <f>+D32*B26*D26</f>
-        <v>9.2223436592166834</v>
+        <v>2.2898109055555831</v>
       </c>
     </row>
     <row r="37" ht="17.25">
@@ -1471,7 +1471,7 @@
         <v>2</v>
       </c>
       <c r="D38">
-        <v>0.089999999999999997</v>
+        <v>0.10000000000000001</v>
       </c>
     </row>
     <row r="39">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="B41" s="6">
         <f>(B38*D38)/F40</f>
-        <v>0.26729999999999998</v>
+        <v>0.29699999999999999</v>
       </c>
       <c r="K41" t="s">
         <v>8</v>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="B42">
         <f>(+SUM(K42:Z42)+(B39*B41)^B39/(FACT(B39)*(1-B41)))^(-1)</f>
-        <v>0.44628556001530151</v>
+        <v>0.40722614982736338</v>
       </c>
       <c r="K42">
         <f t="shared" si="3"/>
@@ -1530,11 +1530,11 @@
       </c>
       <c r="L42">
         <f t="shared" si="4"/>
-        <v>0.80189999999999995</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="M42">
         <f t="shared" si="4"/>
-        <v>0.32152180499999994</v>
+        <v>0.39694050000000003</v>
       </c>
       <c r="N42">
         <f>IF(N43&lt;&gt;0,(($B39*$B41)^N43/(FACT(N43))),0)</f>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="B43">
         <f>+(B39*B41)^B39*B42/(FACT(B39)*(1-B41))</f>
-        <v>0.052347510606872927</v>
+        <v>0.068290799150907425</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -1666,14 +1666,14 @@
       </c>
       <c r="B44" s="6">
         <f>+(B43*D40)/(1-B41)</f>
-        <v>128.6004082057749</v>
+        <v>174.85553125410149</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D44" s="6">
         <f>+B44+B40</f>
-        <v>5528.6004082057752</v>
+        <v>5574.8555312541012</v>
       </c>
     </row>
     <row r="45">
@@ -1682,14 +1682,14 @@
       </c>
       <c r="B45" s="6">
         <f>+B44*B38*D38</f>
-        <v>0.019097160618557568</v>
+        <v>0.028851162656926745</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D45" s="6">
         <f>+D44*B38*D38</f>
-        <v>0.82099716061855743</v>
+        <v>0.91985116265692657</v>
       </c>
     </row>
     <row r="49" ht="17.25">
@@ -2168,7 +2168,7 @@
         <v>2.2898109055555835</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" ht="17.25">
       <c r="A73" s="1" t="s">
         <v>25</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>9.2223436592166834</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="17.25">
       <c r="A85" s="1" t="s">
         <v>27</v>
       </c>
@@ -2439,21 +2439,21 @@
         <v>4</v>
       </c>
       <c r="B88">
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D88">
         <f>+B88/B87</f>
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="E88" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F88">
         <f t="shared" ref="F80:F88" si="11">1/D88</f>
-        <v>0.0011111111111111111</v>
+        <v>0.00083333333333333339</v>
       </c>
     </row>
     <row r="89">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="B89" s="6">
         <f>(B86*D86)/F88</f>
-        <v>0.49500000000000005</v>
+        <v>0.66000000000000003</v>
       </c>
       <c r="K89" t="s">
         <v>8</v>
@@ -2472,17 +2472,13 @@
       <c r="A90" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B90">
-        <f>(+SUM(K90:Z90)+(B87*B89)^B87/(FACT(B87)*(1-B89)))^(-1)</f>
-        <v>0.40400808016160317</v>
-      </c>
       <c r="K90">
         <f t="shared" ref="K82:K90" si="12">($B$3*$B$5)^K91/FACT(K91)</f>
         <v>1</v>
       </c>
       <c r="L90">
         <f t="shared" ref="L82:M90" si="13">IF(L91&lt;&gt;0,(($B87*$B89)^L91/(FACT(L91))),0)</f>
-        <v>0.49500000000000005</v>
+        <v>0.66000000000000003</v>
       </c>
       <c r="M90">
         <f t="shared" si="13"/>
@@ -2547,7 +2543,7 @@
       </c>
       <c r="B91">
         <f>+(B87*B89)^B87*B90/(FACT(B87)*(1-B89))</f>
-        <v>0.39600792015840325</v>
+        <v>0</v>
       </c>
       <c r="K91">
         <v>0</v>
@@ -2617,15 +2613,15 @@
         <v>11</v>
       </c>
       <c r="B92" s="6">
-        <f>+(B91*D88)/(1-B89)</f>
-        <v>705.75668939121385</v>
+        <f>B89*B88/(1-B89)</f>
+        <v>2329.4117647058824</v>
       </c>
       <c r="C92" s="7" t="s">
         <v>12</v>
       </c>
       <c r="D92" s="6">
         <f>+B92+B88</f>
-        <v>1605.756689391214</v>
+        <v>3529.4117647058824</v>
       </c>
     </row>
     <row r="93">
@@ -2633,15 +2629,15 @@
         <v>13</v>
       </c>
       <c r="B93" s="6">
-        <f>+B92*B86*D86</f>
-        <v>0.3881661791651676</v>
+        <f>B92*B86*D86</f>
+        <v>1.2811764705882354</v>
       </c>
       <c r="C93" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D93" s="6">
         <f>+D92*B86*D86</f>
-        <v>0.88316617916516771</v>
+        <v>1.9411764705882353</v>
       </c>
     </row>
     <row r="100">

</xml_diff>